<commit_message>
catching up following live changes made at rehearsal
</commit_message>
<xml_diff>
--- a/DevFiles/hostParamMap.xlsx
+++ b/DevFiles/hostParamMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="0" windowWidth="16080" windowHeight="21240" tabRatio="500"/>
+    <workbookView xWindow="22280" yWindow="0" windowWidth="16080" windowHeight="21240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Parms 1-16</t>
+  </si>
+  <si>
+    <t>tune</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>divergence</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>LFElevel</t>
+  </si>
+  <si>
+    <t>Xshift</t>
+  </si>
+  <si>
+    <t>Yshift</t>
+  </si>
+  <si>
+    <t>RotationAngle</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>InstInsertFX:Sr.Panner</t>
+  </si>
+  <si>
+    <t>PitchLFOmulti</t>
+  </si>
+  <si>
+    <t>curve</t>
+  </si>
+  <si>
+    <t>attack</t>
+  </si>
+  <si>
+    <t>decay</t>
+  </si>
+  <si>
+    <t>sustain</t>
+  </si>
+  <si>
+    <t>release</t>
+  </si>
+  <si>
+    <t>Group:Pitch:ADHSR</t>
+  </si>
+  <si>
+    <t>Group:Source</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>fadein</t>
+  </si>
+  <si>
+    <t>pulseWidth</t>
+  </si>
+  <si>
+    <t>Sine</t>
+  </si>
+  <si>
+    <t>Rectangle</t>
+  </si>
+  <si>
+    <t>Saw</t>
+  </si>
+  <si>
+    <t>dry</t>
+  </si>
+  <si>
+    <t>wet</t>
+  </si>
+  <si>
+    <t>remember: potential to double parameters on one hostAutoNumber</t>
   </si>
 </sst>
 </file>
@@ -70,8 +151,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -80,11 +167,17 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,214 +507,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <f t="shared" ref="A4:A34" si="0">A3+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>